<commit_message>
simrandewangan2710: hlookup and hlookup document add for v and h loopup
</commit_message>
<xml_diff>
--- a/day 12 vlookup and hlookup.xlsx
+++ b/day 12 vlookup and hlookup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data Analytics\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data Analytics\Excel\day 12 vlookup and hlookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE7586F4-D962-4A92-86A9-71D71089E4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66225E9-BA05-479D-935A-740D067D4032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1008,7 +1008,7 @@
   <dimension ref="B1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,12 +1045,30 @@
       <c r="B2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="C2" s="7" t="str">
+        <f>HLOOKUP(C1,$B11:$H13,2,FALSE)</f>
+        <v xml:space="preserve">automotive </v>
+      </c>
+      <c r="D2" s="7" t="str">
+        <f t="shared" ref="D2:H2" si="0">HLOOKUP(D1,$B11:$H13,2,FALSE)</f>
+        <v>offline</v>
+      </c>
+      <c r="E2" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F2" s="7">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="G2" s="7">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="H2" s="7">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
@@ -1102,12 +1120,30 @@
       <c r="B5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="C5" s="7" t="str">
+        <f>HLOOKUP(C1,$B11:$H13,3,FALSE)</f>
+        <v>nandanvan</v>
+      </c>
+      <c r="D5" s="7" t="str">
+        <f t="shared" ref="D5:H5" si="1">HLOOKUP(D1,$B11:$H13,3,FALSE)</f>
+        <v>online</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" si="1"/>
+        <v>15000</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="1"/>
+        <v>200000</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">

</xml_diff>